<commit_message>
Tableau main map with crimes complete, working on secondary data sheets
</commit_message>
<xml_diff>
--- a/CrimeTypeOutcomes_Planning.xlsx
+++ b/CrimeTypeOutcomes_Planning.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t>Outcome</t>
   </si>
@@ -147,6 +148,180 @@
 Evidence of wildlife offences
 Goods on which duty has not been paid etc.
 Seals or hunting equipment</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Court result unavailable</t>
+  </si>
+  <si>
+    <t>Awaiting court outcome</t>
+  </si>
+  <si>
+    <t>Status update unavailable</t>
+  </si>
+  <si>
+    <t>Court case unable to proceed</t>
+  </si>
+  <si>
+    <t>Defendant found not guilty</t>
+  </si>
+  <si>
+    <t>Offender given absolute discharge</t>
+  </si>
+  <si>
+    <t>Unable to prosecute suspect</t>
+  </si>
+  <si>
+    <t>Outcome flag</t>
+  </si>
+  <si>
+    <t>Action to be taken by another organisation</t>
+  </si>
+  <si>
+    <t>Investigation complete; no suspect identified</t>
+  </si>
+  <si>
+    <t>Formal action is not in the public interest</t>
+  </si>
+  <si>
+    <t>Further investigation is not in the public interes</t>
+  </si>
+  <si>
+    <t>Local resolution</t>
+  </si>
+  <si>
+    <t>Offender deprived of property</t>
+  </si>
+  <si>
+    <t>Offender fined</t>
+  </si>
+  <si>
+    <t>Offender given a caution</t>
+  </si>
+  <si>
+    <t>Offender given a drugs possession warning</t>
+  </si>
+  <si>
+    <t>Offender given community sentence</t>
+  </si>
+  <si>
+    <t>Offender given conditional discharge</t>
+  </si>
+  <si>
+    <t>Offender given penalty notice</t>
+  </si>
+  <si>
+    <t>Offender given suspended prison sentence</t>
+  </si>
+  <si>
+    <t>Offender ordered to pay compensation</t>
+  </si>
+  <si>
+    <t>Offender otherwise dealt with</t>
+  </si>
+  <si>
+    <t>Offender sent to prison</t>
+  </si>
+  <si>
+    <t>Suspect charged as part of another case</t>
+  </si>
+  <si>
+    <t>Under investigation</t>
+  </si>
+  <si>
+    <t>Arrest</t>
+  </si>
+  <si>
+    <t>Article found - Detailed outcome unavailable</t>
+  </si>
+  <si>
+    <t>Caution (simple or conditional)</t>
+  </si>
+  <si>
+    <t>Community resolution</t>
+  </si>
+  <si>
+    <t>Khat or Cannabis warning</t>
+  </si>
+  <si>
+    <t>Offender cautioned</t>
+  </si>
+  <si>
+    <t>Offender given drugs possession warning</t>
+  </si>
+  <si>
+    <t>Penalty Notice for Disorder</t>
+  </si>
+  <si>
+    <t>Summons / charged by post</t>
+  </si>
+  <si>
+    <t>Suspect arrested</t>
+  </si>
+  <si>
+    <t>Suspect summonsed to court</t>
+  </si>
+  <si>
+    <t>Suspected psychoactive substances seized - No further action</t>
+  </si>
+  <si>
+    <t>A no further action disposal</t>
+  </si>
+  <si>
+    <t>Nothing found - no further action</t>
+  </si>
+  <si>
+    <t>Crime type</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>OG Outcome</t>
+  </si>
+  <si>
+    <t>Detailed object of search unavailable</t>
+  </si>
+  <si>
+    <t>Evidence of offences under the Act</t>
+  </si>
+  <si>
+    <t>Evidence of wildlife offences</t>
+  </si>
+  <si>
+    <t>Goods on which duty has not been paid etc.</t>
+  </si>
+  <si>
+    <t>Seals or hunting equipment</t>
+  </si>
+  <si>
+    <t>Possession of weapons</t>
+  </si>
+  <si>
+    <t>Public disorder and weapons</t>
+  </si>
+  <si>
+    <t>Game or poaching equipment</t>
+  </si>
+  <si>
+    <t>Violence and sexual offences</t>
+  </si>
+  <si>
+    <t>Violent crime</t>
+  </si>
+  <si>
+    <t>Robbery</t>
+  </si>
+  <si>
+    <t>Theft from the person</t>
+  </si>
+  <si>
+    <t>Criminal damage</t>
+  </si>
+  <si>
+    <t>Fireworks</t>
   </si>
 </sst>
 </file>
@@ -199,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +404,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,4 +831,491 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>